<commit_message>
checked all amplitude data
</commit_message>
<xml_diff>
--- a/UUVDatabase.xlsx
+++ b/UUVDatabase.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Propeller" sheetId="1" state="visible" r:id="rId2"/>
@@ -1441,7 +1441,7 @@
     <t xml:space="preserve">https://www.researchgate.net/publication/233379444_Design_Fabrication_and_Hydrodynamic_Analysis_of_a_Biomimetic_Robot_Fish</t>
   </si>
   <si>
-    <t xml:space="preserve">Univesrity of Washington Robotic Fish</t>
+    <t xml:space="preserve">University of Washington Robotic Fish</t>
   </si>
   <si>
     <t xml:space="preserve">Morgansen</t>
@@ -7786,12 +7786,12 @@
   </sheetPr>
   <dimension ref="A1:AD105"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="D68" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U3" activeCellId="0" sqref="U3"/>
+      <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A68" activeCellId="0" sqref="A68"/>
+      <selection pane="bottomRight" activeCell="M96" activeCellId="0" sqref="M96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7806,9 +7806,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="8" style="1" width="10.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="14.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="19.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="16" style="1" width="19.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="23.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="13.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="11.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="10.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="7.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="20" style="1" width="18.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="13.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="12.5"/>
@@ -8008,7 +8010,7 @@
         <v>4</v>
       </c>
       <c r="S3" s="1" t="n">
-        <v>0.0025</v>
+        <v>0.013</v>
       </c>
       <c r="T3" s="1" t="n">
         <f aca="false">N3*I3/0.000001</f>
@@ -8016,7 +8018,7 @@
       </c>
       <c r="U3" s="1" t="n">
         <f aca="false">(4*PI()*R3*S3*I3^2)/0.000001</f>
-        <v>1158.11671581934</v>
+        <v>6022.20692226058</v>
       </c>
       <c r="AD3" s="1" t="s">
         <v>287</v>
@@ -8070,7 +8072,7 @@
         <v>2.5</v>
       </c>
       <c r="S4" s="1" t="n">
-        <v>0.025</v>
+        <v>0.01299</v>
       </c>
       <c r="T4" s="1" t="n">
         <f aca="false">N4*I4/0.000001</f>
@@ -8078,7 +8080,7 @@
       </c>
       <c r="U4" s="1" t="n">
         <f aca="false">(4*PI()*R4*S4*I4^2)/0.000001</f>
-        <v>16741.54725098</v>
+        <v>8698.90795160921</v>
       </c>
       <c r="V4" s="1" t="n">
         <v>0.057</v>
@@ -8135,7 +8137,7 @@
         <v>1.6</v>
       </c>
       <c r="S5" s="1" t="n">
-        <v>0.02</v>
+        <v>0.026</v>
       </c>
       <c r="T5" s="1" t="n">
         <f aca="false">N5*I5/0.000001</f>
@@ -8143,7 +8145,7 @@
       </c>
       <c r="U5" s="1" t="n">
         <f aca="false">(4*PI()*R5*S5*I5^2)/0.000001</f>
-        <v>11621.3795441594</v>
+        <v>15107.7934074072</v>
       </c>
       <c r="AD5" s="1" t="s">
         <v>297</v>
@@ -8201,7 +8203,7 @@
         <v>7</v>
       </c>
       <c r="S6" s="1" t="n">
-        <v>0.014</v>
+        <v>0.0187</v>
       </c>
       <c r="T6" s="1" t="n">
         <f aca="false">N6*I6/0.000001</f>
@@ -8209,7 +8211,7 @@
       </c>
       <c r="U6" s="1" t="n">
         <f aca="false">(4*PI()*R6*S6*I6^2)/0.000001</f>
-        <v>224538.951199058</v>
+        <v>299919.884815885</v>
       </c>
       <c r="AD6" s="1" t="s">
         <v>302</v>
@@ -8328,17 +8330,10 @@
       <c r="R8" s="1" t="n">
         <v>3.1</v>
       </c>
-      <c r="S8" s="1" t="n">
-        <v>0.0016</v>
-      </c>
       <c r="T8" s="1" t="n">
         <f aca="false">N8*I8/0.000001</f>
         <v>5400</v>
       </c>
-      <c r="U8" s="1" t="n">
-        <f aca="false">(4*PI()*R8*S8*I8^2)/0.000001</f>
-        <v>897.54045475999</v>
-      </c>
       <c r="W8" s="1" t="n">
         <v>0.4</v>
       </c>
@@ -8412,17 +8407,10 @@
       <c r="R9" s="1" t="n">
         <v>3.5</v>
       </c>
-      <c r="S9" s="1" t="n">
-        <v>0.025</v>
-      </c>
       <c r="T9" s="1" t="n">
         <f aca="false">N9*I9/0.000001</f>
         <v>14800</v>
       </c>
-      <c r="U9" s="1" t="n">
-        <f aca="false">(4*PI()*R9*S9*I9^2)/0.000001</f>
-        <v>24084.7059194808</v>
-      </c>
       <c r="AD9" s="1" t="s">
         <v>314</v>
       </c>
@@ -8485,18 +8473,10 @@
       <c r="R10" s="1" t="n">
         <v>1.4</v>
       </c>
-      <c r="S10" s="1" t="n">
-        <f aca="false">ROUND(TAN(RADIANS(30))*(I10/3),2)</f>
-        <v>0.09</v>
-      </c>
       <c r="T10" s="1" t="n">
         <f aca="false">N10*I10/0.000001</f>
         <v>110450</v>
       </c>
-      <c r="U10" s="1" t="n">
-        <f aca="false">(4*PI()*R10*S10*I10^2)/0.000001</f>
-        <v>349764.819857704</v>
-      </c>
       <c r="Y10" s="1" t="n">
         <f aca="false">ROUND(40/60,2)</f>
         <v>0.67</v>
@@ -8736,7 +8716,7 @@
         <v>19</v>
       </c>
       <c r="S14" s="1" t="n">
-        <v>0.14</v>
+        <v>0.2</v>
       </c>
       <c r="T14" s="1" t="n">
         <f aca="false">N14*I14/0.000001</f>
@@ -8744,7 +8724,7 @@
       </c>
       <c r="U14" s="1" t="n">
         <f aca="false">(4*PI()*R14*S14*I14^2)/0.000001</f>
-        <v>83566.3645854885</v>
+        <v>119380.520836412</v>
       </c>
       <c r="AD14" s="1" t="s">
         <v>334</v>
@@ -8798,8 +8778,7 @@
         <v>1</v>
       </c>
       <c r="S15" s="1" t="n">
-        <f aca="false">ROUND(TAN(RADIANS(20))*0.06,2)</f>
-        <v>0.02</v>
+        <v>0.074</v>
       </c>
       <c r="T15" s="1" t="n">
         <f aca="false">N15*I15/0.000001</f>
@@ -8807,7 +8786,7 @@
       </c>
       <c r="U15" s="1" t="n">
         <f aca="false">(4*PI()*R15*S15*I15^2)/0.000001</f>
-        <v>21871.7680542921</v>
+        <v>80925.5418008809</v>
       </c>
       <c r="W15" s="1" t="n">
         <v>0.6</v>
@@ -8864,7 +8843,7 @@
         <v>4.7</v>
       </c>
       <c r="S16" s="1" t="n">
-        <v>5E-005</v>
+        <v>0.001296</v>
       </c>
       <c r="T16" s="1" t="n">
         <f aca="false">N16*I16/0.000001</f>
@@ -8872,7 +8851,7 @@
       </c>
       <c r="U16" s="1" t="n">
         <f aca="false">(4*PI()*R16*S16*I16^2)/0.000001</f>
-        <v>8.61123112719577</v>
+        <v>223.203110816914</v>
       </c>
       <c r="AD16" s="1" t="s">
         <v>343</v>
@@ -8992,8 +8971,7 @@
         <v>0.32</v>
       </c>
       <c r="S18" s="1" t="n">
-        <f aca="false">ROUND(TAN(RADIANS(30))*(I18/4),2)</f>
-        <v>0.04</v>
+        <v>0.346</v>
       </c>
       <c r="T18" s="1" t="n">
         <f aca="false">N18*I18/0.000001</f>
@@ -9001,7 +8979,7 @@
       </c>
       <c r="U18" s="1" t="n">
         <f aca="false">(4*PI()*R18*S18*I18^2)/0.000001</f>
-        <v>10873.4291651927</v>
+        <v>94055.1622789169</v>
       </c>
       <c r="AD18" s="1" t="s">
         <v>350</v>
@@ -9055,8 +9033,7 @@
         <v>4.5</v>
       </c>
       <c r="S19" s="1" t="n">
-        <f aca="false">ROUND(TAN(RADIANS(20))*(I19/4),2)</f>
-        <v>0.03</v>
+        <v>0.0784</v>
       </c>
       <c r="T19" s="1" t="n">
         <f aca="false">N19*I19/0.000001</f>
@@ -9064,7 +9041,7 @@
       </c>
       <c r="U19" s="1" t="n">
         <f aca="false">(4*PI()*R19*S19*I19^2)/0.000001</f>
-        <v>156780.050404043</v>
+        <v>409718.531722567</v>
       </c>
       <c r="AD19" s="1" t="s">
         <v>354</v>
@@ -9109,8 +9086,7 @@
         <v>3.125</v>
       </c>
       <c r="S20" s="1" t="n">
-        <f aca="false">ROUND(TAN(RADIANS(15))*0.067,2)</f>
-        <v>0.02</v>
+        <v>0.10654</v>
       </c>
       <c r="T20" s="1" t="n">
         <f aca="false">N20*I20/0.000001</f>
@@ -9118,7 +9094,7 @@
       </c>
       <c r="U20" s="1" t="n">
         <f aca="false">(4*PI()*R20*S20*I20^2)/0.000001</f>
-        <v>89196.8840188848</v>
+        <v>475151.801168599</v>
       </c>
       <c r="Z20" s="1" t="n">
         <v>5</v>
@@ -9214,7 +9190,7 @@
         <v>0</v>
       </c>
       <c r="I22" s="1" t="n">
-        <v>0.117</v>
+        <v>0.167</v>
       </c>
       <c r="J22" s="1" t="n">
         <v>0.026</v>
@@ -9235,15 +9211,15 @@
         <v>2</v>
       </c>
       <c r="S22" s="1" t="n">
-        <v>0.1</v>
+        <v>0.1497</v>
       </c>
       <c r="T22" s="1" t="n">
         <f aca="false">N22*I22/0.000001</f>
-        <v>9360</v>
+        <v>13360</v>
       </c>
       <c r="U22" s="1" t="n">
         <f aca="false">(4*PI()*R22*S22*I22^2)/0.000001</f>
-        <v>34404.2094679925</v>
+        <v>104928.774913121</v>
       </c>
       <c r="AD22" s="1" t="s">
         <v>364</v>
@@ -9291,8 +9267,7 @@
         <v>8</v>
       </c>
       <c r="S23" s="1" t="n">
-        <f aca="false">ROUND(TAN(RADIANS(40))*(I23/4),2)</f>
-        <v>0.05</v>
+        <v>0.20977</v>
       </c>
       <c r="T23" s="1" t="n">
         <f aca="false">N23*I23/0.000001</f>
@@ -9300,7 +9275,7 @@
       </c>
       <c r="U23" s="1" t="n">
         <f aca="false">(4*PI()*R23*S23*I23^2)/0.000001</f>
-        <v>314159.265358979</v>
+        <v>1318023.78188706</v>
       </c>
       <c r="AD23" s="1" t="s">
         <v>368</v>
@@ -9408,7 +9383,7 @@
         <v>1</v>
       </c>
       <c r="S25" s="1" t="n">
-        <v>0.0231</v>
+        <v>0.105</v>
       </c>
       <c r="T25" s="1" t="n">
         <f aca="false">N25*I25/0.000001</f>
@@ -9416,7 +9391,7 @@
       </c>
       <c r="U25" s="1" t="n">
         <f aca="false">(4*PI()*R25*S25*I25^2)/0.000001</f>
-        <v>14049.7050016781</v>
+        <v>63862.2954621733</v>
       </c>
       <c r="AD25" s="1" t="s">
         <v>378</v>
@@ -9632,26 +9607,24 @@
         <v>0.1</v>
       </c>
       <c r="M29" s="1" t="n">
-        <v>0.17</v>
+        <v>0.173</v>
       </c>
       <c r="N29" s="1" t="n">
-        <f aca="false">M29</f>
-        <v>0.17</v>
+        <v>0.173</v>
       </c>
       <c r="R29" s="1" t="n">
         <v>2.4</v>
       </c>
       <c r="S29" s="1" t="n">
-        <f aca="false">0.14*I29</f>
-        <v>0.0448</v>
+        <v>0.141</v>
       </c>
       <c r="T29" s="1" t="n">
         <f aca="false">N29*I29/0.000001</f>
-        <v>54400</v>
+        <v>55360</v>
       </c>
       <c r="U29" s="1" t="n">
         <f aca="false">(4*PI()*R29*S29*I29^2)/0.000001</f>
-        <v>138356.343649884</v>
+        <v>435451.885148072</v>
       </c>
       <c r="AD29" s="1" t="s">
         <v>394</v>
@@ -9757,7 +9730,7 @@
         <v>1</v>
       </c>
       <c r="S31" s="1" t="n">
-        <v>0.006</v>
+        <v>0.089686</v>
       </c>
       <c r="T31" s="1" t="n">
         <f aca="false">N31*I31/0.000001</f>
@@ -9765,7 +9738,7 @@
       </c>
       <c r="U31" s="1" t="n">
         <f aca="false">(4*PI()*R31*S31*I31^2)/0.000001</f>
-        <v>3749.4782656888</v>
+        <v>56045.9512894277</v>
       </c>
       <c r="AD31" s="1" t="s">
         <v>401</v>
@@ -9819,7 +9792,7 @@
         <v>30</v>
       </c>
       <c r="S32" s="1" t="n">
-        <v>0.01</v>
+        <v>0.0471</v>
       </c>
       <c r="T32" s="1" t="n">
         <f aca="false">N32*I32/0.000001</f>
@@ -9827,7 +9800,7 @@
       </c>
       <c r="U32" s="1" t="n">
         <f aca="false">(4*PI()*R32*S32*I32^2)/0.000001</f>
-        <v>339292.006587698</v>
+        <v>1598065.35102806</v>
       </c>
       <c r="V32" s="1" t="n">
         <v>7.5</v>
@@ -9891,10 +9864,10 @@
         <v>0.9944235</v>
       </c>
       <c r="R33" s="1" t="n">
-        <v>15</v>
+        <v>5.8</v>
       </c>
       <c r="S33" s="1" t="n">
-        <v>0.034</v>
+        <v>0.17</v>
       </c>
       <c r="T33" s="1" t="n">
         <f aca="false">N33*I33/0.000001</f>
@@ -9902,7 +9875,7 @@
       </c>
       <c r="U33" s="1" t="n">
         <f aca="false">(4*PI()*R33*S33*I33^2)/0.000001</f>
-        <v>416735.40709134</v>
+        <v>805688.453709923</v>
       </c>
       <c r="Y33" s="1" t="n">
         <v>1.16</v>
@@ -10056,18 +10029,10 @@
       <c r="R36" s="1" t="n">
         <v>0.4</v>
       </c>
-      <c r="S36" s="1" t="n">
-        <f aca="false">ROUND(TAN(0.4)*I36,2)</f>
-        <v>0.05</v>
-      </c>
       <c r="T36" s="1" t="n">
         <f aca="false">N36*I36/0.000001</f>
         <v>960</v>
       </c>
-      <c r="U36" s="1" t="n">
-        <f aca="false">(4*PI()*R36*S36*I36^2)/0.000001</f>
-        <v>3619.11473693544</v>
-      </c>
       <c r="AD36" s="1" t="s">
         <v>419</v>
       </c>
@@ -10460,8 +10425,7 @@
         <v>2.5</v>
       </c>
       <c r="S42" s="1" t="n">
-        <f aca="false">ROUND(TAN(RADIANS(50))*(I42/2),2)</f>
-        <v>0.3</v>
+        <v>0.18198</v>
       </c>
       <c r="T42" s="1" t="n">
         <f aca="false">N42*I42/0.000001</f>
@@ -10469,7 +10433,7 @@
       </c>
       <c r="U42" s="1" t="n">
         <f aca="false">(4*PI()*R42*S42*I42^2)/0.000001</f>
-        <v>2356194.49019234</v>
+        <v>1429267.57775068</v>
       </c>
       <c r="W42" s="1" t="n">
         <f aca="false">0.52*I42</f>
@@ -10517,9 +10481,6 @@
       <c r="R43" s="1" t="n">
         <v>1.2</v>
       </c>
-      <c r="S43" s="1" t="n">
-        <v>0.099</v>
-      </c>
       <c r="AD43" s="1" t="s">
         <v>439</v>
       </c>
@@ -10623,7 +10584,7 @@
         <v>9</v>
       </c>
       <c r="S45" s="1" t="n">
-        <v>0.0005</v>
+        <v>0.00877</v>
       </c>
       <c r="T45" s="1" t="n">
         <f aca="false">N45*I45/0.000001</f>
@@ -10631,7 +10592,7 @@
       </c>
       <c r="U45" s="1" t="n">
         <f aca="false">(4*PI()*R45*S45*I45^2)/0.000001</f>
-        <v>183.726621567238</v>
+        <v>3222.56494228936</v>
       </c>
       <c r="AD45" s="1" t="s">
         <v>447</v>
@@ -10681,7 +10642,7 @@
         <v>1.4</v>
       </c>
       <c r="S46" s="1" t="n">
-        <v>0.0004</v>
+        <v>0.001</v>
       </c>
       <c r="T46" s="1" t="n">
         <f aca="false">N46*I46/0.000001</f>
@@ -10689,7 +10650,7 @@
       </c>
       <c r="U46" s="1" t="n">
         <f aca="false">(4*PI()*R46*S46*I46^2)/0.000001</f>
-        <v>1125.94680704658</v>
+        <v>2814.86701761645</v>
       </c>
       <c r="AD46" s="1" t="s">
         <v>450</v>
@@ -10743,7 +10704,7 @@
         <v>0.8</v>
       </c>
       <c r="S47" s="1" t="n">
-        <v>0.266</v>
+        <v>0.11083</v>
       </c>
       <c r="T47" s="1" t="n">
         <f aca="false">N47*I47/0.000001</f>
@@ -10751,7 +10712,7 @@
       </c>
       <c r="U47" s="1" t="n">
         <f aca="false">(4*PI()*R47*S47*I47^2)/0.000001</f>
-        <v>15402952.3203972</v>
+        <v>6417703.78071288</v>
       </c>
       <c r="V47" s="1" t="n">
         <v>1.9</v>
@@ -10798,18 +10759,10 @@
       <c r="R48" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="S48" s="1" t="n">
-        <f aca="false">ROUND(TAN(RADIANS(50))*(I48/3),2)</f>
-        <v>0.24</v>
-      </c>
       <c r="T48" s="1" t="n">
         <f aca="false">N48*I48/0.000001</f>
         <v>300000</v>
       </c>
-      <c r="U48" s="1" t="n">
-        <f aca="false">(4*PI()*R48*S48*I48^2)/0.000001</f>
-        <v>2171468.84216126</v>
-      </c>
       <c r="AD48" s="1" t="s">
         <v>456</v>
       </c>
@@ -10910,7 +10863,7 @@
         <v>6.6</v>
       </c>
       <c r="S50" s="1" t="n">
-        <v>0.044</v>
+        <v>0.176</v>
       </c>
       <c r="T50" s="1" t="n">
         <f aca="false">N50*I50/0.000001</f>
@@ -10918,7 +10871,7 @@
       </c>
       <c r="U50" s="1" t="n">
         <f aca="false">(4*PI()*R50*S50*I50^2)/0.000001</f>
-        <v>228079.626650619</v>
+        <v>912318.506602476</v>
       </c>
       <c r="AD50" s="1" t="s">
         <v>461</v>
@@ -10972,7 +10925,7 @@
         <v>20</v>
       </c>
       <c r="S51" s="1" t="n">
-        <v>0.063</v>
+        <v>0.196875</v>
       </c>
       <c r="T51" s="1" t="n">
         <f aca="false">N51*I51/0.000001</f>
@@ -10980,7 +10933,7 @@
       </c>
       <c r="U51" s="1" t="n">
         <f aca="false">(4*PI()*R51*S51*I51^2)/0.000001</f>
-        <v>1621363.40214708</v>
+        <v>5066760.63170962</v>
       </c>
       <c r="AD51" s="1" t="s">
         <v>463</v>
@@ -11140,8 +11093,7 @@
         <v>1.9</v>
       </c>
       <c r="S54" s="1" t="n">
-        <f aca="false">ROUND(TAN(RADIANS(30))*(I54/3),2)</f>
-        <v>0.1</v>
+        <v>0.11647</v>
       </c>
       <c r="T54" s="1" t="n">
         <f aca="false">N54*I54/0.000001</f>
@@ -11149,7 +11101,7 @@
       </c>
       <c r="U54" s="1" t="n">
         <f aca="false">(4*PI()*R54*S54*I54^2)/0.000001</f>
-        <v>703466.050283809</v>
+        <v>819326.908765552</v>
       </c>
       <c r="AD54" s="1" t="s">
         <v>475</v>
@@ -11292,7 +11244,7 @@
         <v>1</v>
       </c>
       <c r="I57" s="1" t="n">
-        <v>0.2</v>
+        <v>0.11</v>
       </c>
       <c r="J57" s="1" t="n">
         <v>0.02</v>
@@ -11313,15 +11265,15 @@
         <v>23</v>
       </c>
       <c r="S57" s="1" t="n">
-        <v>0.012</v>
+        <v>0.1454</v>
       </c>
       <c r="T57" s="1" t="n">
         <f aca="false">N57*I57/0.000001</f>
-        <v>45000</v>
+        <v>24750</v>
       </c>
       <c r="U57" s="1" t="n">
         <f aca="false">(4*PI()*R57*S57*I57^2)/0.000001</f>
-        <v>138732.731582525</v>
+        <v>508495.924963333</v>
       </c>
       <c r="AD57" s="1" t="s">
         <v>484</v>
@@ -11551,18 +11503,10 @@
       <c r="R61" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="S61" s="1" t="n">
-        <f aca="false">ROUND(TAN(RADIANS(30))*(I61/3),2)</f>
-        <v>0.13</v>
-      </c>
       <c r="T61" s="1" t="n">
         <f aca="false">N61*I61/0.000001</f>
         <v>218130</v>
       </c>
-      <c r="U61" s="1" t="n">
-        <f aca="false">(4*PI()*R61*S61*I61^2)/0.000001</f>
-        <v>1427532.91595107</v>
-      </c>
       <c r="W61" s="1" t="n">
         <v>0.1</v>
       </c>
@@ -11669,18 +11613,10 @@
       <c r="R63" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="S63" s="1" t="n">
-        <f aca="false">ROUND(TAN(RADIANS(40))*(I63/3),2)</f>
-        <v>0.13</v>
-      </c>
       <c r="T63" s="1" t="n">
         <f aca="false">N63*I63/0.000001</f>
         <v>174800</v>
       </c>
-      <c r="U63" s="1" t="n">
-        <f aca="false">(4*PI()*R63*S63*I63^2)/0.000001</f>
-        <v>691351.445719584</v>
-      </c>
       <c r="W63" s="1" t="n">
         <v>0.36</v>
       </c>
@@ -12079,8 +12015,7 @@
         <v>5</v>
       </c>
       <c r="S70" s="1" t="n">
-        <f aca="false">ROUND(TAN(RADIANS(45))*0.01,2)</f>
-        <v>0.01</v>
+        <v>0.1558</v>
       </c>
       <c r="T70" s="1" t="n">
         <f aca="false">N70*I70/0.000001</f>
@@ -12088,7 +12023,7 @@
       </c>
       <c r="U70" s="1" t="n">
         <f aca="false">(4*PI()*R70*S70*I70^2)/0.000001</f>
-        <v>1005.30964914873</v>
+        <v>15662.7243337373</v>
       </c>
       <c r="AD70" s="1" t="s">
         <v>525</v>
@@ -12141,17 +12076,10 @@
       <c r="R71" s="1" t="n">
         <v>0.8</v>
       </c>
-      <c r="S71" s="1" t="n">
-        <v>0.0826</v>
-      </c>
       <c r="T71" s="1" t="n">
         <f aca="false">N71*I71/0.000001</f>
         <v>6165</v>
       </c>
-      <c r="U71" s="1" t="n">
-        <f aca="false">(4*PI()*R71*S71*I71^2)/0.000001</f>
-        <v>18683.6798294292</v>
-      </c>
       <c r="AD71" s="1" t="s">
         <v>529</v>
       </c>
@@ -12324,7 +12252,7 @@
         <v>1.5</v>
       </c>
       <c r="S74" s="1" t="n">
-        <v>0.072</v>
+        <v>0.0836</v>
       </c>
       <c r="T74" s="1" t="n">
         <f aca="false">N74*I74/0.000001</f>
@@ -12332,7 +12260,7 @@
       </c>
       <c r="U74" s="1" t="n">
         <f aca="false">(4*PI()*R74*S74*I74^2)/0.000001</f>
-        <v>665012.332911887</v>
+        <v>772153.208769914</v>
       </c>
       <c r="AD74" s="1" t="s">
         <v>539</v>
@@ -12453,18 +12381,10 @@
       <c r="R76" s="1" t="n">
         <v>6.2</v>
       </c>
-      <c r="S76" s="1" t="n">
-        <f aca="false">ROUND(TAN(RADIANS(45))*I76,2)</f>
-        <v>0.61</v>
-      </c>
       <c r="T76" s="1" t="n">
         <f aca="false">N76*I76/0.000001</f>
         <v>282440</v>
       </c>
-      <c r="U76" s="1" t="n">
-        <f aca="false">(4*PI()*R76*S76*I76^2)/0.000001</f>
-        <v>17917117.0470873</v>
-      </c>
       <c r="AD76" s="1" t="s">
         <v>545</v>
       </c>
@@ -12516,18 +12436,10 @@
       <c r="R77" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="S77" s="1" t="n">
-        <f aca="false">ROUND(TAN(RADIANS(30))*I77,2)</f>
-        <v>0.23</v>
-      </c>
       <c r="T77" s="1" t="n">
         <f aca="false">N77*I77/0.000001</f>
         <v>128000</v>
       </c>
-      <c r="U77" s="1" t="n">
-        <f aca="false">(4*PI()*R77*S77*I77^2)/0.000001</f>
-        <v>924884.877216836</v>
-      </c>
       <c r="V77" s="1" t="n">
         <f aca="false">ROUND(DEGREES(1),2)</f>
         <v>57.3</v>
@@ -12707,8 +12619,7 @@
         <v>1.5</v>
       </c>
       <c r="S80" s="1" t="n">
-        <f aca="false">ROUND(0.1*I80,2)</f>
-        <v>0.06</v>
+        <v>0.1</v>
       </c>
       <c r="T80" s="1" t="n">
         <f aca="false">N80*I80/0.000001</f>
@@ -12716,7 +12627,7 @@
       </c>
       <c r="U80" s="1" t="n">
         <f aca="false">(4*PI()*R80*S80*I80^2)/0.000001</f>
-        <v>391027.25175219</v>
+        <v>651712.08625365</v>
       </c>
       <c r="AD80" s="1" t="s">
         <v>559</v>
@@ -12952,7 +12863,7 @@
         <v>1.67</v>
       </c>
       <c r="S84" s="1" t="n">
-        <v>0.1</v>
+        <v>0.099</v>
       </c>
       <c r="T84" s="1" t="n">
         <f aca="false">N84*I84/0.000001</f>
@@ -12960,7 +12871,7 @@
       </c>
       <c r="U84" s="1" t="n">
         <f aca="false">(4*PI()*R84*S84*I84^2)/0.000001</f>
-        <v>768134.169288176</v>
+        <v>760452.827595295</v>
       </c>
       <c r="Z84" s="1" t="n">
         <v>6</v>
@@ -13112,18 +13023,10 @@
       <c r="R87" s="1" t="n">
         <v>2.6</v>
       </c>
-      <c r="S87" s="1" t="n">
-        <f aca="false">ROUND(TAN(RADIANS(40))*0.136,2)</f>
-        <v>0.11</v>
-      </c>
       <c r="T87" s="1" t="n">
         <f aca="false">N87*I87/0.000001</f>
         <v>236720</v>
       </c>
-      <c r="U87" s="1" t="n">
-        <f aca="false">(4*PI()*R87*S87*I87^2)/0.000001</f>
-        <v>695794.914368822</v>
-      </c>
       <c r="Z87" s="1" t="n">
         <v>11.1</v>
       </c>
@@ -13191,17 +13094,10 @@
       <c r="R88" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="S88" s="1" t="n">
-        <v>0.31</v>
-      </c>
       <c r="T88" s="1" t="n">
         <f aca="false">N88*I88/0.000001</f>
         <v>1936000</v>
       </c>
-      <c r="U88" s="1" t="n">
-        <f aca="false">(4*PI()*R88*S88*I88^2)/0.000001</f>
-        <v>24133865.5613242</v>
-      </c>
       <c r="W88" s="1" t="n">
         <v>1.75</v>
       </c>
@@ -13380,17 +13276,10 @@
       <c r="R91" s="1" t="n">
         <v>1.25</v>
       </c>
-      <c r="S91" s="1" t="n">
-        <v>0.35</v>
-      </c>
       <c r="T91" s="1" t="n">
         <f aca="false">N91*I91/0.000001</f>
         <v>1131000</v>
       </c>
-      <c r="U91" s="1" t="n">
-        <f aca="false">(4*PI()*R91*S91*I91^2)/0.000001</f>
-        <v>9291260.27299181</v>
-      </c>
       <c r="AD91" s="1" t="s">
         <v>599</v>
       </c>
@@ -13447,7 +13336,7 @@
         <v>1</v>
       </c>
       <c r="S92" s="1" t="n">
-        <v>0.3</v>
+        <v>0.3658</v>
       </c>
       <c r="T92" s="1" t="n">
         <f aca="false">N92*I92/0.000001</f>
@@ -13455,7 +13344,7 @@
       </c>
       <c r="U92" s="1" t="n">
         <f aca="false">(4*PI()*R92*S92*I92^2)/0.000001</f>
-        <v>2534888.28032853</v>
+        <v>3090873.77648059</v>
       </c>
       <c r="V92" s="1" t="n">
         <v>15</v>
@@ -13506,25 +13395,25 @@
         <v>0.1</v>
       </c>
       <c r="M93" s="1" t="n">
-        <v>0.03</v>
+        <v>0.052</v>
       </c>
       <c r="N93" s="1" t="n">
         <f aca="false">M93</f>
-        <v>0.03</v>
+        <v>0.052</v>
       </c>
       <c r="R93" s="1" t="n">
-        <v>0.5</v>
+        <v>1.57</v>
       </c>
       <c r="S93" s="1" t="n">
-        <v>0.0396</v>
+        <v>0.0043</v>
       </c>
       <c r="T93" s="1" t="n">
         <f aca="false">N93*I93/0.000001</f>
-        <v>9000</v>
+        <v>15600</v>
       </c>
       <c r="U93" s="1" t="n">
         <f aca="false">(4*PI()*R93*S93*I93^2)/0.000001</f>
-        <v>22393.272434788</v>
+        <v>7635.20112157849</v>
       </c>
       <c r="AD93" s="1" t="s">
         <v>607</v>
@@ -13620,7 +13509,7 @@
         <v>1.5</v>
       </c>
       <c r="S95" s="1" t="n">
-        <v>0.125</v>
+        <v>0.22</v>
       </c>
       <c r="T95" s="1" t="n">
         <f aca="false">N95*I95/0.000001</f>
@@ -13628,7 +13517,7 @@
       </c>
       <c r="U95" s="1" t="n">
         <f aca="false">(4*PI()*R95*S95*I95^2)/0.000001</f>
-        <v>415632.70806993</v>
+        <v>731513.566203076</v>
       </c>
       <c r="AD95" s="1" t="s">
         <v>612</v>
@@ -13675,8 +13564,7 @@
         <v>0.42504</v>
       </c>
       <c r="N96" s="1" t="n">
-        <f aca="false">M96</f>
-        <v>0.42504</v>
+        <v>0.043478</v>
       </c>
       <c r="R96" s="1" t="n">
         <v>2</v>
@@ -13687,7 +13575,7 @@
       </c>
       <c r="T96" s="1" t="n">
         <f aca="false">N96*I96/0.000001</f>
-        <v>215070.24</v>
+        <v>21999.868</v>
       </c>
       <c r="U96" s="1" t="n">
         <f aca="false">(4*PI()*R96*S96*I96^2)/0.000001</f>
@@ -13753,18 +13641,10 @@
       <c r="R97" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="S97" s="1" t="n">
-        <f aca="false">ROUND(TAN(RADIANS(30))*0.36,2)</f>
-        <v>0.21</v>
-      </c>
       <c r="T97" s="1" t="n">
         <f aca="false">N97*I97/0.000001</f>
         <v>77760</v>
       </c>
-      <c r="U97" s="1" t="n">
-        <f aca="false">(4*PI()*R97*S97*I97^2)/0.000001</f>
-        <v>1900035.23689111</v>
-      </c>
       <c r="AD97" s="1" t="s">
         <v>619</v>
       </c>
@@ -13813,17 +13693,10 @@
       <c r="R98" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="S98" s="1" t="n">
-        <v>0.2886</v>
-      </c>
       <c r="T98" s="1" t="n">
         <f aca="false">N98*I98/0.000001</f>
         <v>561000</v>
       </c>
-      <c r="U98" s="1" t="n">
-        <f aca="false">(4*PI()*R98*S98*I98^2)/0.000001</f>
-        <v>4388252.01675791</v>
-      </c>
       <c r="AA98" s="1" t="n">
         <v>0.6</v>
       </c>
@@ -13880,17 +13753,10 @@
       <c r="R99" s="1" t="n">
         <v>0.55</v>
       </c>
-      <c r="S99" s="1" t="n">
-        <v>0.11</v>
-      </c>
       <c r="T99" s="1" t="n">
         <f aca="false">N99*I99/0.000001</f>
         <v>131100</v>
       </c>
-      <c r="U99" s="1" t="n">
-        <f aca="false">(4*PI()*R99*S99*I99^2)/0.000001</f>
-        <v>988040.942650481</v>
-      </c>
       <c r="AD99" s="1" t="s">
         <v>625</v>
       </c>
@@ -14085,7 +13951,7 @@
         <v>2.093</v>
       </c>
       <c r="S102" s="1" t="n">
-        <v>0.46185</v>
+        <v>0.125</v>
       </c>
       <c r="T102" s="1" t="n">
         <f aca="false">N102*I102/0.000001</f>
@@ -14093,7 +13959,7 @@
       </c>
       <c r="U102" s="1" t="n">
         <f aca="false">(4*PI()*R102*S102*I102^2)/0.000001</f>
-        <v>31097108.2635009</v>
+        <v>8416452.3826732</v>
       </c>
       <c r="AD102" s="1" t="s">
         <v>635</v>
@@ -14323,12 +14189,12 @@
   </sheetPr>
   <dimension ref="A1:AC41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="H1" activeCellId="0" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R6" activeCellId="0" sqref="R6"/>
+      <selection pane="bottomRight" activeCell="R41" activeCellId="0" sqref="R41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14888,17 +14754,9 @@
       <c r="Q9" s="9" t="n">
         <v>1.8</v>
       </c>
-      <c r="R9" s="9" t="n">
-        <f aca="false">ROUND(TAN(RADIANS(10))*0.1,2)</f>
-        <v>0.02</v>
-      </c>
       <c r="S9" s="9" t="n">
         <f aca="false">(H9*M9)/0.000001</f>
         <v>79200</v>
-      </c>
-      <c r="T9" s="9" t="n">
-        <f aca="false">(4*PI()*Q9*R9*H9^2)/0.000001</f>
-        <v>49265.1993565337</v>
       </c>
       <c r="U9" s="9" t="n">
         <v>260</v>
@@ -15121,18 +14979,10 @@
       <c r="Q13" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="R13" s="9" t="n">
-        <f aca="false">ROUND(TAN(RADIANS(40))*0.165,2)</f>
-        <v>0.14</v>
-      </c>
       <c r="S13" s="9" t="n">
         <f aca="false">(H13*M13)/0.000001</f>
         <v>436590</v>
       </c>
-      <c r="T13" s="9" t="n">
-        <f aca="false">(4*PI()*Q13*R13*H13^2)/0.000001</f>
-        <v>6158679.21509699</v>
-      </c>
       <c r="U13" s="9" t="n">
         <v>55</v>
       </c>
@@ -15187,8 +15037,7 @@
         <v>1</v>
       </c>
       <c r="R14" s="9" t="n">
-        <f aca="false">ROUND(TAN(RADIANS(40))*0.1,2)</f>
-        <v>0.08</v>
+        <v>0.095</v>
       </c>
       <c r="S14" s="9" t="n">
         <f aca="false">(H14*M14)/0.000001</f>
@@ -15196,7 +15045,7 @@
       </c>
       <c r="T14" s="9" t="n">
         <f aca="false">(4*PI()*Q14*R14*H14^2)/0.000001</f>
-        <v>784183.990615593</v>
+        <v>931218.488856016</v>
       </c>
       <c r="Y14" s="11"/>
       <c r="AC14" s="12" t="s">
@@ -15303,8 +15152,7 @@
         <v>1.5</v>
       </c>
       <c r="R16" s="9" t="n">
-        <f aca="false">ROUND(TAN(RADIANS(39.5))*(I16/3),2)</f>
-        <v>0.11</v>
+        <v>0.12674</v>
       </c>
       <c r="S16" s="9" t="n">
         <f aca="false">(H16*M16)/0.000001</f>
@@ -15312,7 +15160,7 @@
       </c>
       <c r="T16" s="9" t="n">
         <f aca="false">(4*PI()*Q16*R16*H16^2)/0.000001</f>
-        <v>1327008.73687633</v>
+        <v>1528955.33919733</v>
       </c>
       <c r="Y16" s="11"/>
       <c r="AC16" s="12" t="s">
@@ -15365,8 +15213,7 @@
         <v>2</v>
       </c>
       <c r="R17" s="9" t="n">
-        <f aca="false">ROUND(TAN(RADIANS(40))*0.2,2)</f>
-        <v>0.17</v>
+        <v>0.3356</v>
       </c>
       <c r="S17" s="9" t="n">
         <f aca="false">(H17*M17)/0.000001</f>
@@ -15374,7 +15221,7 @@
       </c>
       <c r="T17" s="9" t="n">
         <f aca="false">(4*PI()*Q17*R17*H17^2)/0.000001</f>
-        <v>1068141.50222053</v>
+        <v>2108636.98908947</v>
       </c>
       <c r="V17" s="10" t="n">
         <v>3</v>
@@ -15525,26 +15372,25 @@
         <v>4</v>
       </c>
       <c r="L20" s="9" t="n">
-        <v>0.48</v>
+        <v>0.3</v>
       </c>
       <c r="M20" s="9" t="n">
         <f aca="false">L20</f>
-        <v>0.48</v>
+        <v>0.3</v>
       </c>
       <c r="Q20" s="9" t="n">
         <v>0.5</v>
       </c>
       <c r="R20" s="9" t="n">
-        <f aca="false">ROUND(TAN(RADIANS(40))*(I20/2),2)</f>
-        <v>0.35</v>
+        <v>0.38</v>
       </c>
       <c r="S20" s="9" t="n">
         <f aca="false">(H20*M20)/0.000001</f>
-        <v>220800</v>
+        <v>138000</v>
       </c>
       <c r="T20" s="9" t="n">
         <f aca="false">(4*PI()*Q20*R20*H20^2)/0.000001</f>
-        <v>465332.70384972</v>
+        <v>505218.364179696</v>
       </c>
       <c r="Y20" s="11"/>
       <c r="AC20" s="9" t="s">
@@ -15597,8 +15443,7 @@
         <v>0.8</v>
       </c>
       <c r="R21" s="9" t="n">
-        <f aca="false">ROUND(TAN(RADIANS(40))*(I21/2),2)</f>
-        <v>0.25</v>
+        <v>0.45</v>
       </c>
       <c r="S21" s="9" t="n">
         <f aca="false">(H21*M21)/0.000001</f>
@@ -15606,7 +15451,7 @@
       </c>
       <c r="T21" s="9" t="n">
         <f aca="false">(4*PI()*Q21*R21*H21^2)/0.000001</f>
-        <v>628318.530717959</v>
+        <v>1130973.35529233</v>
       </c>
       <c r="Y21" s="11"/>
       <c r="AC21" s="9" t="s">
@@ -15658,18 +15503,10 @@
       <c r="Q22" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="R22" s="9" t="n">
-        <f aca="false">ROUND(TAN(RADIANS(20))*(I22/2),2)</f>
-        <v>0.16</v>
-      </c>
       <c r="S22" s="9" t="n">
         <f aca="false">(H22*M22)/0.000001</f>
         <v>403000</v>
       </c>
-      <c r="T22" s="9" t="n">
-        <f aca="false">(4*PI()*Q22*R22*H22^2)/0.000001</f>
-        <v>1698973.30706136</v>
-      </c>
       <c r="Y22" s="11"/>
       <c r="AC22" s="9" t="s">
         <v>713</v>
@@ -15782,7 +15619,7 @@
         <v>1.2</v>
       </c>
       <c r="R24" s="9" t="n">
-        <v>0.052</v>
+        <v>0.18857</v>
       </c>
       <c r="S24" s="9" t="n">
         <f aca="false">(H24*M24)/0.000001</f>
@@ -15790,7 +15627,7 @@
       </c>
       <c r="T24" s="9" t="n">
         <f aca="false">(4*PI()*Q24*R24*H24^2)/0.000001</f>
-        <v>384229.347904646</v>
+        <v>1393348.61796883</v>
       </c>
       <c r="Y24" s="11"/>
       <c r="AC24" s="9" t="s">
@@ -15903,7 +15740,7 @@
         <v>1.28</v>
       </c>
       <c r="R26" s="9" t="n">
-        <v>0.057</v>
+        <v>0.42857</v>
       </c>
       <c r="S26" s="9" t="n">
         <f aca="false">(H26*M26)/0.000001</f>
@@ -15911,7 +15748,7 @@
       </c>
       <c r="T26" s="9" t="n">
         <f aca="false">(4*PI()*Q26*R26*H26^2)/0.000001</f>
-        <v>16218.0252140183</v>
+        <v>121939.632736348</v>
       </c>
       <c r="V26" s="10" t="n">
         <v>0.118</v>
@@ -16021,7 +15858,7 @@
         <v>1.25</v>
       </c>
       <c r="R28" s="9" t="n">
-        <v>0.00275</v>
+        <v>0.01527</v>
       </c>
       <c r="S28" s="9" t="n">
         <f aca="false">(H28*M28)/0.000001</f>
@@ -16029,7 +15866,7 @@
       </c>
       <c r="T28" s="9" t="n">
         <f aca="false">(4*PI()*Q28*R28*H28^2)/0.000001</f>
-        <v>1399.57952717425</v>
+        <v>7771.48341089122</v>
       </c>
       <c r="Y28" s="11"/>
       <c r="AC28" s="9" t="s">
@@ -16138,18 +15975,10 @@
       <c r="Q30" s="9" t="n">
         <v>1.5</v>
       </c>
-      <c r="R30" s="9" t="n">
-        <f aca="false">ROUND(TAN(RADIANS(40))*0.43,2)</f>
-        <v>0.36</v>
-      </c>
       <c r="S30" s="9" t="n">
         <f aca="false">(H30*M30)/0.000001</f>
         <v>111000</v>
       </c>
-      <c r="T30" s="9" t="n">
-        <f aca="false">(4*PI()*Q30*R30*H30^2)/0.000001</f>
-        <v>928981.514037116</v>
-      </c>
       <c r="V30" s="10" t="n">
         <v>0.01</v>
       </c>
@@ -16203,18 +16032,10 @@
       <c r="Q31" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="R31" s="9" t="n">
-        <f aca="false">ROUND(TAN(RADIANS(45))*(I31/2),2)</f>
-        <v>0.25</v>
-      </c>
       <c r="S31" s="9" t="n">
         <f aca="false">(H31*M31)/0.000001</f>
         <v>39000</v>
       </c>
-      <c r="T31" s="9" t="n">
-        <f aca="false">(4*PI()*Q31*R31*H31^2)/0.000001</f>
-        <v>282743.338823081</v>
-      </c>
       <c r="Y31" s="11"/>
       <c r="AC31" s="9" t="s">
         <v>738</v>
@@ -16266,7 +16087,7 @@
         <v>10</v>
       </c>
       <c r="R32" s="9" t="n">
-        <v>0.04</v>
+        <v>0.1533</v>
       </c>
       <c r="S32" s="9" t="n">
         <f aca="false">(H32*M32)/0.000001</f>
@@ -16274,7 +16095,7 @@
       </c>
       <c r="T32" s="9" t="n">
         <f aca="false">(4*PI()*Q32*R32*H32^2)/0.000001</f>
-        <v>113097.335529233</v>
+        <v>433445.538415784</v>
       </c>
       <c r="Y32" s="11"/>
       <c r="AC32" s="9" t="s">
@@ -16381,7 +16202,7 @@
         <v>0.4</v>
       </c>
       <c r="R34" s="9" t="n">
-        <v>0.015</v>
+        <v>0.107</v>
       </c>
       <c r="S34" s="9" t="n">
         <f aca="false">(H34*M34)/0.000001</f>
@@ -16389,7 +16210,7 @@
       </c>
       <c r="T34" s="9" t="n">
         <f aca="false">(4*PI()*Q34*R34*H34^2)/0.000001</f>
-        <v>1477.80518424864</v>
+        <v>10541.6769809736</v>
       </c>
       <c r="Y34" s="11"/>
       <c r="AC34" s="9" t="s">
@@ -16439,7 +16260,7 @@
         <v>10</v>
       </c>
       <c r="R35" s="9" t="n">
-        <v>0.025</v>
+        <v>0.2272</v>
       </c>
       <c r="S35" s="9" t="n">
         <f aca="false">(H35*M35)/0.000001</f>
@@ -16447,7 +16268,7 @@
       </c>
       <c r="T35" s="9" t="n">
         <f aca="false">(4*PI()*Q35*R35*H35^2)/0.000001</f>
-        <v>38013.2711084365</v>
+        <v>345464.607833471</v>
       </c>
       <c r="Y35" s="11"/>
       <c r="AC35" s="9" t="s">
@@ -16564,7 +16385,7 @@
         <v>0.5</v>
       </c>
       <c r="R37" s="9" t="n">
-        <v>0.3</v>
+        <v>0.35211</v>
       </c>
       <c r="S37" s="9" t="n">
         <f aca="false">(H37*M37)/0.000001</f>
@@ -16572,7 +16393,7 @@
       </c>
       <c r="T37" s="9" t="n">
         <f aca="false">(4*PI()*Q37*R37*H37^2)/0.000001</f>
-        <v>950206.114004769</v>
+        <v>1115256.9160074</v>
       </c>
       <c r="Y37" s="11"/>
       <c r="AC37" s="9" t="s">
@@ -16625,8 +16446,7 @@
         <v>0.157</v>
       </c>
       <c r="R38" s="9" t="n">
-        <f aca="false">0.2*0.1</f>
-        <v>0.02</v>
+        <v>0.010332</v>
       </c>
       <c r="S38" s="9" t="n">
         <f aca="false">(H38*M38)/0.000001</f>
@@ -16634,7 +16454,7 @@
       </c>
       <c r="T38" s="9" t="n">
         <f aca="false">(4*PI()*Q38*R38*H38^2)/0.000001</f>
-        <v>1740.11560445277</v>
+        <v>898.943721260302</v>
       </c>
       <c r="Y38" s="11"/>
       <c r="AC38" s="9" t="s">
@@ -16697,8 +16517,7 @@
         <v>0.167</v>
       </c>
       <c r="R39" s="9" t="n">
-        <f aca="false">0.45*0.085</f>
-        <v>0.03825</v>
+        <v>0.20238</v>
       </c>
       <c r="S39" s="9" t="n">
         <f aca="false">(H39*M39)/0.000001</f>
@@ -16706,7 +16525,7 @@
       </c>
       <c r="T39" s="9" t="n">
         <f aca="false">(4*PI()*Q39*R39*H39^2)/0.000001</f>
-        <v>971.277090091661</v>
+        <v>5139.00803902615</v>
       </c>
       <c r="Y39" s="11"/>
       <c r="AC39" s="9" t="s">

</xml_diff>

<commit_message>
added segregation for robot-sw plot
</commit_message>
<xml_diff>
--- a/UUVDatabase.xlsx
+++ b/UUVDatabase.xlsx
@@ -2779,12 +2779,19 @@
     <cellStyle name="Text 13" xfId="29"/>
     <cellStyle name="Warning 14" xfId="30"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFCFCFC"/>
-          <bgColor rgb="FF1B1E20"/>
+          <fgColor rgb="00FFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFFFFFFF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -7787,11 +7794,11 @@
   <dimension ref="A1:AD105"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D68" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A68" activeCellId="0" sqref="A68"/>
-      <selection pane="bottomRight" activeCell="M96" activeCellId="0" sqref="M96"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8137,7 +8144,7 @@
         <v>1.6</v>
       </c>
       <c r="S5" s="1" t="n">
-        <v>0.026</v>
+        <v>0.25</v>
       </c>
       <c r="T5" s="1" t="n">
         <f aca="false">N5*I5/0.000001</f>
@@ -8145,7 +8152,7 @@
       </c>
       <c r="U5" s="1" t="n">
         <f aca="false">(4*PI()*R5*S5*I5^2)/0.000001</f>
-        <v>15107.7934074072</v>
+        <v>145267.244301992</v>
       </c>
       <c r="AD5" s="1" t="s">
         <v>297</v>
@@ -8871,7 +8878,7 @@
         <v>338</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>296</v>
+        <v>342</v>
       </c>
       <c r="F17" s="1" t="n">
         <v>1</v>
@@ -8892,7 +8899,7 @@
         <v>0.122</v>
       </c>
       <c r="N17" s="1" t="n">
-        <v>0.7</v>
+        <v>0.69</v>
       </c>
       <c r="O17" s="2" t="n">
         <f aca="false">P17/L17</f>
@@ -8906,18 +8913,18 @@
         <v>1.331424</v>
       </c>
       <c r="R17" s="1" t="n">
-        <v>2.75</v>
+        <v>1.75</v>
       </c>
       <c r="S17" s="1" t="n">
         <v>0.1</v>
       </c>
       <c r="T17" s="1" t="n">
         <f aca="false">N17*I17/0.000001</f>
-        <v>84000</v>
+        <v>82800</v>
       </c>
       <c r="U17" s="1" t="n">
         <f aca="false">(4*PI()*R17*S17*I17^2)/0.000001</f>
-        <v>49762.8276328623</v>
+        <v>31667.2539481851</v>
       </c>
       <c r="AD17" s="1" t="s">
         <v>347</v>

</xml_diff>